<commit_message>
Minor modification of southeast_asia data
</commit_message>
<xml_diff>
--- a/southeast_asia/distance.xlsx
+++ b/southeast_asia/distance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/energy/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PhD\PREP-SHOT modelling\PREP-SHOT-main\southeast_asia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F6C4931-F2A6-4B4F-A682-7B4680F0FDDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2802B84-DFF8-4462-BE1A-F84107BC4F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{91ADC8C9-FE2E-FA4B-A60E-EA27C07434CB}"/>
+    <workbookView xWindow="-25710" yWindow="-2420" windowWidth="25820" windowHeight="15500" xr2:uid="{91ADC8C9-FE2E-FA4B-A60E-EA27C07434CB}"/>
   </bookViews>
   <sheets>
     <sheet name="distance" sheetId="1" r:id="rId1"/>
@@ -205,9 +205,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0_ "/>
+    <numFmt numFmtId="176" formatCode="0_ "/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -235,6 +235,12 @@
       <name val="Noto Sans CJK SC"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -258,15 +264,15 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -282,9 +288,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 主题">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -322,7 +328,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -428,7 +434,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -570,7 +576,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -581,10 +587,10 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5" customWidth="1"/>
@@ -625,16 +631,20 @@
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
       <c r="C3" s="2">
-        <v>655.248103745506</v>
-      </c>
-      <c r="D3" s="1"/>
+        <v>655</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1293</v>
+      </c>
       <c r="E3" s="2">
-        <v>498.80441732870793</v>
+        <v>499</v>
       </c>
       <c r="F3" s="2">
-        <v>462.72930653266542</v>
+        <v>463</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -642,65 +652,84 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>655.248103745506</v>
-      </c>
-      <c r="C4" s="1"/>
+        <v>655</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
       <c r="D4" s="2">
-        <v>813.47046378915729</v>
+        <v>813</v>
       </c>
       <c r="E4" s="2">
-        <v>477.14405006718567</v>
+        <v>477</v>
       </c>
       <c r="F4" s="2">
-        <v>338.91069144222269</v>
+        <v>339</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1">
+        <v>1293</v>
+      </c>
       <c r="C5" s="2">
-        <v>813.47046378915729</v>
-      </c>
-      <c r="D5" s="1"/>
+        <v>813</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
       <c r="E5" s="2">
-        <v>820.30154138586408</v>
-      </c>
-      <c r="F5" s="1"/>
+        <v>820</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1144</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="2">
-        <v>498.80441732870793</v>
+        <v>499</v>
       </c>
       <c r="C6" s="2">
-        <v>477.14405006718567</v>
+        <v>477</v>
       </c>
       <c r="D6" s="2">
-        <v>820.30154138586408</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+        <v>820</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>591</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="2">
-        <v>462.72930653266542</v>
+        <v>463</v>
       </c>
       <c r="C7" s="2">
-        <v>338.91069144222269</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+        <v>339</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1144</v>
+      </c>
+      <c r="E7" s="1">
+        <v>591</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <phoneticPr fontId="4" type="noConversion"/>
+  <dataValidations xWindow="26" yWindow="444" count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Unit" prompt="m" sqref="A1" xr:uid="{00000000-0002-0000-0400-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>